<commit_message>
fix FC - first IF statement to check non-batter out, move batter; ELSE is to check batter
</commit_message>
<xml_diff>
--- a/donaj_2016.xlsx
+++ b/donaj_2016.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="72" windowWidth="21060" windowHeight="10080"/>
+    <workbookView xWindow="384" yWindow="72" windowWidth="21060" windowHeight="10080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="donaj_2016" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing Run_Scored" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">donaj_2016!$A$1:$AL$156</definedName>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="261">
   <si>
     <t>Rk</t>
   </si>
@@ -491,6 +492,315 @@
   </si>
   <si>
     <t>W9-0</t>
+  </si>
+  <si>
+    <t>game_id</t>
+  </si>
+  <si>
+    <t>this_half</t>
+  </si>
+  <si>
+    <t>stat_type</t>
+  </si>
+  <si>
+    <t>stat_value</t>
+  </si>
+  <si>
+    <t>actual_play</t>
+  </si>
+  <si>
+    <t>TOR201604080</t>
+  </si>
+  <si>
+    <t>4_1</t>
+  </si>
+  <si>
+    <t>runs_scored</t>
+  </si>
+  <si>
+    <t>HR/7/F.3-H;2-H;1-H</t>
+  </si>
+  <si>
+    <t>TOR201604090</t>
+  </si>
+  <si>
+    <t>1_1</t>
+  </si>
+  <si>
+    <t>HR/7/L.1-H</t>
+  </si>
+  <si>
+    <t>3_1</t>
+  </si>
+  <si>
+    <t>HR/78/L.2-H</t>
+  </si>
+  <si>
+    <t>TOR201604100</t>
+  </si>
+  <si>
+    <t>64(1)/FO/G.3-H;2-H(UR)(E4/TH)(NR)</t>
+  </si>
+  <si>
+    <t>8_1</t>
+  </si>
+  <si>
+    <t>HR/78/F</t>
+  </si>
+  <si>
+    <t>TOR201604120</t>
+  </si>
+  <si>
+    <t>D8/F.3-H;1-H</t>
+  </si>
+  <si>
+    <t>TOR201604130</t>
+  </si>
+  <si>
+    <t>D8/L.3-H</t>
+  </si>
+  <si>
+    <t>TOR201604140</t>
+  </si>
+  <si>
+    <t>5_1</t>
+  </si>
+  <si>
+    <t>HR/8/F.3-H;2-H</t>
+  </si>
+  <si>
+    <t>TOR201604230</t>
+  </si>
+  <si>
+    <t>S5/G.3-H;2-3;1-2</t>
+  </si>
+  <si>
+    <t>2_1</t>
+  </si>
+  <si>
+    <t>TOR201604240</t>
+  </si>
+  <si>
+    <t>S8/L-.2-H;1-2</t>
+  </si>
+  <si>
+    <t>HR/78/L.1-H</t>
+  </si>
+  <si>
+    <t>TOR201604250</t>
+  </si>
+  <si>
+    <t>D9/L.2-H;1-H</t>
+  </si>
+  <si>
+    <t>TOR201605050</t>
+  </si>
+  <si>
+    <t>D8/L+.3-H;2-H;1-H</t>
+  </si>
+  <si>
+    <t>HR/78/F.2-H;1-H</t>
+  </si>
+  <si>
+    <t>S8/L.2-H;1-2</t>
+  </si>
+  <si>
+    <t>TOR201605060</t>
+  </si>
+  <si>
+    <t>6_1</t>
+  </si>
+  <si>
+    <t>HR/78/F.1-H</t>
+  </si>
+  <si>
+    <t>TOR201605270</t>
+  </si>
+  <si>
+    <t>HR/89/F</t>
+  </si>
+  <si>
+    <t>HR/9/F.1-H</t>
+  </si>
+  <si>
+    <t>TOR201605300</t>
+  </si>
+  <si>
+    <t>D7/L+.1-H</t>
+  </si>
+  <si>
+    <t>TOR201606010</t>
+  </si>
+  <si>
+    <t>7_1</t>
+  </si>
+  <si>
+    <t>D9/L+.2-H;1-3</t>
+  </si>
+  <si>
+    <t>TOR201606090</t>
+  </si>
+  <si>
+    <t>D9/L.2-H</t>
+  </si>
+  <si>
+    <t>TOR201606110</t>
+  </si>
+  <si>
+    <t>9/L/SF.3-H;2-3</t>
+  </si>
+  <si>
+    <t>TOR201606120</t>
+  </si>
+  <si>
+    <t>S8/G.2-H</t>
+  </si>
+  <si>
+    <t>TOR201606140</t>
+  </si>
+  <si>
+    <t>S8/L.2-H;1-3</t>
+  </si>
+  <si>
+    <t>HR/8/L.1-H</t>
+  </si>
+  <si>
+    <t>TOR201606220</t>
+  </si>
+  <si>
+    <t>TOR201606300</t>
+  </si>
+  <si>
+    <t>HR/8/F</t>
+  </si>
+  <si>
+    <t>TOR201607020</t>
+  </si>
+  <si>
+    <t>HR/8/F.2-H;1-H</t>
+  </si>
+  <si>
+    <t>D7/L.3-H;2-H</t>
+  </si>
+  <si>
+    <t>TOR201607030</t>
+  </si>
+  <si>
+    <t>S7/G.3-H;2-3</t>
+  </si>
+  <si>
+    <t>D7/L.2-H</t>
+  </si>
+  <si>
+    <t>TOR201607050</t>
+  </si>
+  <si>
+    <t>HR/8/L</t>
+  </si>
+  <si>
+    <t>S9/F-.2-H</t>
+  </si>
+  <si>
+    <t>7/F/SF.3-H</t>
+  </si>
+  <si>
+    <t>TOR201607070</t>
+  </si>
+  <si>
+    <t>S8/L+.2-H</t>
+  </si>
+  <si>
+    <t>S9/G.3-H;2-H;1-3</t>
+  </si>
+  <si>
+    <t>TOR201607100</t>
+  </si>
+  <si>
+    <t>TOR201607260</t>
+  </si>
+  <si>
+    <t>HR/8/F.1-H</t>
+  </si>
+  <si>
+    <t>TOR201607300</t>
+  </si>
+  <si>
+    <t>W.3-H;2-3;1-2</t>
+  </si>
+  <si>
+    <t>TOR201608100</t>
+  </si>
+  <si>
+    <t>HR/7/L.2-H(UR);1-H(UR);B-H(UR)</t>
+  </si>
+  <si>
+    <t>TOR201608130</t>
+  </si>
+  <si>
+    <t>TOR201608230</t>
+  </si>
+  <si>
+    <t>164(1)3/GDP.3-H;2-3</t>
+  </si>
+  <si>
+    <t>TOR201608240</t>
+  </si>
+  <si>
+    <t>S7/G.3-H;1-2</t>
+  </si>
+  <si>
+    <t>TOR201608250</t>
+  </si>
+  <si>
+    <t>TOR201608260</t>
+  </si>
+  <si>
+    <t>HR/89/F.1-H</t>
+  </si>
+  <si>
+    <t>TOR201608270</t>
+  </si>
+  <si>
+    <t>TOR201608280</t>
+  </si>
+  <si>
+    <t>HR/7/F</t>
+  </si>
+  <si>
+    <t>TOR201609100</t>
+  </si>
+  <si>
+    <t>S6/L-.3-H(UR);1-2</t>
+  </si>
+  <si>
+    <t>TOR201609110</t>
+  </si>
+  <si>
+    <t>TOR201609230</t>
+  </si>
+  <si>
+    <t>S7/L.3-H(UR);2-H(UR);1-2</t>
+  </si>
+  <si>
+    <t>HR/7/F.2-H</t>
+  </si>
+  <si>
+    <t>TOR201609240</t>
+  </si>
+  <si>
+    <t>HR/7/L.2-H;1-H</t>
+  </si>
+  <si>
+    <t>TOR201609250</t>
+  </si>
+  <si>
+    <t>S8/L.3-H</t>
+  </si>
+  <si>
+    <t>TOR201609260</t>
+  </si>
+  <si>
+    <t>TOR201609270</t>
   </si>
 </sst>
 </file>
@@ -975,9 +1285,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1323,9 +1634,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AL156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:L153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18270,4 +18581,2104 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43563</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43564</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43565</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43567</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43568</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43569</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43577</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43579</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>43580</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>43581</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>43582</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>43588</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>43589</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>43590</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>43591</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>43592</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>43601</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43602</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>43612</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>43613</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>43614</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>43615</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>43616</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>43625</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>43626</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>43627</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>43628</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>43629</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>43630</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>43637</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>43638</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>43646</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>43648</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>43649</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>43650</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>43651</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>43652</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>43653</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>43654</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>43655</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>43656</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>43668</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>43669</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>43670</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>43671</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I51" s="2">
+        <v>1</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>43672</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>43673</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I53" s="2">
+        <v>1</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>43675</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I54" s="2">
+        <v>1</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>43676</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I56" s="2">
+        <v>1</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>43685</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I57" s="2">
+        <v>1</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>43686</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I58" s="2">
+        <v>1</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>43687</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I59" s="2">
+        <v>1</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>43689</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I60" s="2">
+        <v>1</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>43690</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I61" s="2">
+        <v>1</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>43691</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I62" s="2">
+        <v>1</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>43700</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>43701</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I64" s="2">
+        <v>1</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>43702</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I65" s="2">
+        <v>1</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>43703</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I66" s="2">
+        <v>1</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>43704</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>43705</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>43717</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>43718</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>43719</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>43731</v>
+      </c>
+      <c r="B72">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>43732</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>43733</v>
+      </c>
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>43734</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>43735</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>43736</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>43737</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>